<commit_message>
modified:   NewFile.xlsx 	modified:   grade.py 	modified:   mycsv23.xlsx
</commit_message>
<xml_diff>
--- a/NewFile.xlsx
+++ b/NewFile.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
   <si>
     <t>Student_Number</t>
   </si>
@@ -173,61 +173,286 @@
     <t>Flag indicating whether this grade should be excluded from honor roll (1=yes)</t>
   </si>
   <si>
-    <t>HS Arabic Non-Native Foundation 3</t>
+    <t>Nature of Science DP2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>GEMS American Academy</t>
+  </si>
+  <si>
+    <t>Used when calculating graduation requirements</t>
+  </si>
+  <si>
+    <t>Broderick; Matthew</t>
+  </si>
+  <si>
+    <t>DP 2 Math Studies</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Baker; Kelli</t>
+  </si>
+  <si>
+    <t>DP 2 History HL</t>
+  </si>
+  <si>
+    <t>Fatu; Alexandra</t>
+  </si>
+  <si>
+    <t>DP 2 Music HL</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>Holland; Dave</t>
+  </si>
+  <si>
+    <t>DP 2 English Language and Literature HL</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>Sciolis; Catherine</t>
+  </si>
+  <si>
+    <t>DP 2 Theory of Knowledge</t>
+  </si>
+  <si>
+    <t>DP 1 English Language and Literature HL</t>
+  </si>
+  <si>
+    <t>2600</t>
+  </si>
+  <si>
+    <t>Van Pelt; George</t>
+  </si>
+  <si>
+    <t>DP 1 Math Studies</t>
+  </si>
+  <si>
+    <t>DP 1 Nature of Science SL</t>
+  </si>
+  <si>
+    <t>DP 1 History HL</t>
+  </si>
+  <si>
+    <t>DP 1 Music HL</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>HS Arabic Non-Native Foundation 2</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>Hassan; Mohamed</t>
+  </si>
+  <si>
+    <t>English 10</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometry                                </t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>Sami; Farah</t>
+  </si>
+  <si>
+    <t>Physics 1</t>
+  </si>
+  <si>
+    <t>Perez; Elizabeth</t>
+  </si>
+  <si>
+    <t>World Studies 10</t>
+  </si>
+  <si>
+    <t>Risner; Kelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS Accomplished Visual Arts             </t>
+  </si>
+  <si>
+    <t>Hull; Andrew</t>
+  </si>
+  <si>
+    <t>HS Spanish Phase 1/2</t>
+  </si>
+  <si>
+    <t>Gil; Carmen</t>
+  </si>
+  <si>
+    <t>Physical Education 10</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>Lovett; Gerard</t>
+  </si>
+  <si>
+    <t>Arabic 9 Standard</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>2400</t>
+  </si>
+  <si>
+    <t>Mohammad Awad; Samah</t>
+  </si>
+  <si>
+    <t>UAE Social Studies 9 English</t>
+  </si>
+  <si>
+    <t>English 9</t>
+  </si>
+  <si>
+    <t>Sharif; Korosh</t>
+  </si>
+  <si>
+    <t>Algebra 1 9</t>
+  </si>
+  <si>
+    <t>Liebhart; Robert</t>
+  </si>
+  <si>
+    <t>Biology 9</t>
+  </si>
+  <si>
+    <t>Shakarchi; Kamila</t>
+  </si>
+  <si>
+    <t>World Geography 9</t>
+  </si>
+  <si>
+    <t>Visual Arts 9</t>
+  </si>
+  <si>
+    <t>Spanish Foundation 9</t>
+  </si>
+  <si>
+    <t>Beck; Cynthia</t>
+  </si>
+  <si>
+    <t>Physical Education 9</t>
+  </si>
+  <si>
+    <t>Samuela; Steluta</t>
+  </si>
+  <si>
+    <t>Freshmen Experiece 9</t>
   </si>
   <si>
     <t>A+</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>2700</t>
-  </si>
-  <si>
-    <t>GEMS American Academy</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Daoud; Hiba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creative Writing                        </t>
-  </si>
-  <si>
-    <t>Sciolis; Catherine</t>
-  </si>
-  <si>
-    <t>HS French Phase 2/3</t>
-  </si>
-  <si>
-    <t>B-</t>
-  </si>
-  <si>
-    <t>Lajoie; Michele</t>
-  </si>
-  <si>
-    <t>Algebra 2</t>
-  </si>
-  <si>
-    <t>C+</t>
-  </si>
-  <si>
-    <t>Addo; Ataa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historical Studies: US History          </t>
-  </si>
-  <si>
-    <t>A-</t>
-  </si>
-  <si>
-    <t>Jamieson; Kelly</t>
+    <t>Masters; Kim</t>
+  </si>
+  <si>
+    <t>UAE Social Studies 8 English</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>Leite Oliveira Da Silva; Renan</t>
+  </si>
+  <si>
+    <t>Arabic 8 Language Acquisition</t>
+  </si>
+  <si>
+    <t>Alhashash; Sadiya</t>
+  </si>
+  <si>
+    <t>English 8</t>
+  </si>
+  <si>
+    <t>Peltier; Ben</t>
+  </si>
+  <si>
+    <t>Intro to Algebra 8</t>
+  </si>
+  <si>
+    <t>Science 8</t>
+  </si>
+  <si>
+    <t>Livesey; Paul</t>
+  </si>
+  <si>
+    <t>20th Century History &amp; Geography 8</t>
+  </si>
+  <si>
+    <t>Visual Arts 8</t>
+  </si>
+  <si>
+    <t>Music - Instrumental 8</t>
+  </si>
+  <si>
+    <t>Robertson; Jared</t>
+  </si>
+  <si>
+    <t>Spanish C 8</t>
+  </si>
+  <si>
+    <t>Liebhart; Stephanie</t>
+  </si>
+  <si>
+    <t>Physical Education 8</t>
+  </si>
+  <si>
+    <t>Information Technology 8</t>
+  </si>
+  <si>
+    <t>Singh; Abhishek</t>
+  </si>
+  <si>
+    <t>UAE Social Studies 7 English</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>G7 Arabic</t>
+  </si>
+  <si>
+    <t>G7 English Creative Writing</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Pre Algebra 7</t>
+  </si>
+  <si>
+    <t>Science 7</t>
+  </si>
+  <si>
+    <t>G7 World History &amp; Geography 2</t>
+  </si>
+  <si>
+    <t>G7/8 Visual Arts 1</t>
   </si>
 </sst>
 </file>
@@ -1044,13 +1269,13 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" t="n">
-        <v>609136</v>
+        <v>605410</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>97307</v>
+        <v>70001</v>
       </c>
       <c r="D7" t="n">
         <v>0.5</v>
@@ -1068,22 +1293,22 @@
         <v>55</v>
       </c>
       <c r="I7" t="n">
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
         <v>56</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="n">
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
         <v>57</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>58</v>
-      </c>
-      <c r="N7" t="s">
-        <v>59</v>
       </c>
       <c r="O7" t="n">
         <v>3</v>
@@ -1120,19 +1345,19 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" t="n">
-        <v>609136</v>
+        <v>605410</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="n">
-        <v>97307</v>
+        <v>70001</v>
       </c>
       <c r="D8" t="n">
         <v>0.5</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F8" t="n">
         <v>0.5</v>
@@ -1144,20 +1369,18 @@
         <v>55</v>
       </c>
       <c r="I8" t="n">
-        <v>4.3</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K8" t="s">
         <v>56</v>
       </c>
-      <c r="L8" t="s">
-        <v>57</v>
-      </c>
-      <c r="M8" t="s">
-        <v>58</v>
-      </c>
+      <c r="L8" t="n">
+        <v>12</v>
+      </c>
+      <c r="M8" t="s"/>
       <c r="N8" t="s">
         <v>61</v>
       </c>
@@ -1195,24 +1418,58 @@
       <c r="AL8" t="s"/>
     </row>
     <row r="9" spans="1:38">
-      <c r="A9" t="s"/>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
-      <c r="E9" t="s"/>
-      <c r="F9" t="s"/>
-      <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
-      <c r="J9" t="s"/>
-      <c r="K9" t="s"/>
-      <c r="L9" t="s"/>
+      <c r="A9" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>86</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="n">
+        <v>12</v>
+      </c>
       <c r="M9" t="s"/>
-      <c r="N9" t="s"/>
-      <c r="O9" t="s"/>
-      <c r="P9" t="s"/>
-      <c r="Q9" t="s"/>
-      <c r="R9" t="s"/>
+      <c r="N9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
       <c r="S9" t="s"/>
       <c r="T9" t="s"/>
       <c r="U9" t="s"/>
@@ -1236,19 +1493,19 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="n">
-        <v>609136</v>
+        <v>605410</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C10" t="n">
-        <v>97307</v>
+        <v>70001</v>
       </c>
       <c r="D10" t="n">
         <v>0.5</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F10" t="n">
         <v>0.5</v>
@@ -1260,22 +1517,20 @@
         <v>55</v>
       </c>
       <c r="I10" t="n">
-        <v>2.7</v>
+        <v>2.2</v>
       </c>
       <c r="J10" t="n">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s">
         <v>56</v>
       </c>
-      <c r="L10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" t="s">
-        <v>58</v>
-      </c>
+      <c r="L10" t="n">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s"/>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O10" t="n">
         <v>3</v>
@@ -1312,22 +1567,22 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" t="n">
-        <v>609136</v>
+        <v>605410</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" t="n">
-        <v>97307</v>
+        <v>70001</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
@@ -1336,22 +1591,20 @@
         <v>55</v>
       </c>
       <c r="I11" t="n">
-        <v>2.3</v>
+        <v>3.8</v>
       </c>
       <c r="J11" t="n">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
         <v>56</v>
       </c>
-      <c r="L11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" t="s">
-        <v>58</v>
-      </c>
+      <c r="L11" t="n">
+        <v>12</v>
+      </c>
+      <c r="M11" t="s"/>
       <c r="N11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O11" t="n">
         <v>3</v>
@@ -1388,19 +1641,19 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" t="n">
-        <v>609136</v>
+        <v>605410</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>97307</v>
+        <v>70001</v>
       </c>
       <c r="D12" t="n">
         <v>0.5</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F12" t="n">
         <v>0.5</v>
@@ -1412,22 +1665,20 @@
         <v>55</v>
       </c>
       <c r="I12" t="n">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="J12" t="n">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K12" t="s">
         <v>56</v>
       </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" t="s">
-        <v>58</v>
-      </c>
+      <c r="L12" t="n">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s"/>
       <c r="N12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="O12" t="n">
         <v>3</v>
@@ -1463,24 +1714,58 @@
       <c r="AL12" t="s"/>
     </row>
     <row r="13" spans="1:38">
-      <c r="A13" t="s"/>
-      <c r="B13" t="s"/>
-      <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
-      <c r="F13" t="s"/>
-      <c r="G13" t="s"/>
-      <c r="H13" t="s"/>
-      <c r="I13" t="s"/>
-      <c r="J13" t="s"/>
-      <c r="K13" t="s"/>
-      <c r="L13" t="s"/>
+      <c r="A13" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>86</v>
+      </c>
+      <c r="K13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" t="n">
+        <v>11</v>
+      </c>
       <c r="M13" t="s"/>
-      <c r="N13" t="s"/>
-      <c r="O13" t="s"/>
-      <c r="P13" t="s"/>
-      <c r="Q13" t="s"/>
-      <c r="R13" t="s"/>
+      <c r="N13" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
       <c r="S13" t="s"/>
       <c r="T13" t="s"/>
       <c r="U13" t="s"/>
@@ -1503,24 +1788,58 @@
       <c r="AL13" t="s"/>
     </row>
     <row r="14" spans="1:38">
-      <c r="A14" t="s"/>
-      <c r="B14" t="s"/>
-      <c r="C14" t="s"/>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
-      <c r="F14" t="s"/>
-      <c r="G14" t="s"/>
-      <c r="H14" t="s"/>
-      <c r="I14" t="s"/>
-      <c r="J14" t="s"/>
-      <c r="K14" t="s"/>
-      <c r="L14" t="s"/>
+      <c r="A14" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" t="n">
+        <v>86</v>
+      </c>
+      <c r="K14" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" t="n">
+        <v>11</v>
+      </c>
       <c r="M14" t="s"/>
-      <c r="N14" t="s"/>
-      <c r="O14" t="s"/>
-      <c r="P14" t="s"/>
-      <c r="Q14" t="s"/>
-      <c r="R14" t="s"/>
+      <c r="N14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O14" t="n">
+        <v>3</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
       <c r="S14" t="s"/>
       <c r="T14" t="s"/>
       <c r="U14" t="s"/>
@@ -1543,24 +1862,58 @@
       <c r="AL14" t="s"/>
     </row>
     <row r="15" spans="1:38">
-      <c r="A15" t="s"/>
-      <c r="B15" t="s"/>
-      <c r="C15" t="s"/>
-      <c r="D15" t="s"/>
-      <c r="E15" t="s"/>
-      <c r="F15" t="s"/>
-      <c r="G15" t="s"/>
-      <c r="H15" t="s"/>
-      <c r="I15" t="s"/>
-      <c r="J15" t="s"/>
-      <c r="K15" t="s"/>
-      <c r="L15" t="s"/>
+      <c r="A15" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="J15" t="n">
+        <v>86</v>
+      </c>
+      <c r="K15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" t="n">
+        <v>11</v>
+      </c>
       <c r="M15" t="s"/>
-      <c r="N15" t="s"/>
-      <c r="O15" t="s"/>
-      <c r="P15" t="s"/>
-      <c r="Q15" t="s"/>
-      <c r="R15" t="s"/>
+      <c r="N15" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" t="n">
+        <v>3</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
       <c r="S15" t="s"/>
       <c r="T15" t="s"/>
       <c r="U15" t="s"/>
@@ -1583,24 +1936,58 @@
       <c r="AL15" t="s"/>
     </row>
     <row r="16" spans="1:38">
-      <c r="A16" t="s"/>
-      <c r="B16" t="s"/>
-      <c r="C16" t="s"/>
-      <c r="D16" t="s"/>
-      <c r="E16" t="s"/>
-      <c r="F16" t="s"/>
-      <c r="G16" t="s"/>
-      <c r="H16" t="s"/>
-      <c r="I16" t="s"/>
-      <c r="J16" t="s"/>
-      <c r="K16" t="s"/>
-      <c r="L16" t="s"/>
+      <c r="A16" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>89</v>
+      </c>
+      <c r="K16" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" t="n">
+        <v>11</v>
+      </c>
       <c r="M16" t="s"/>
-      <c r="N16" t="s"/>
-      <c r="O16" t="s"/>
-      <c r="P16" t="s"/>
-      <c r="Q16" t="s"/>
-      <c r="R16" t="s"/>
+      <c r="N16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
       <c r="S16" t="s"/>
       <c r="T16" t="s"/>
       <c r="U16" t="s"/>
@@ -1623,24 +2010,58 @@
       <c r="AL16" t="s"/>
     </row>
     <row r="17" spans="1:38">
-      <c r="A17" t="s"/>
-      <c r="B17" t="s"/>
-      <c r="C17" t="s"/>
-      <c r="D17" t="s"/>
-      <c r="E17" t="s"/>
-      <c r="F17" t="s"/>
-      <c r="G17" t="s"/>
-      <c r="H17" t="s"/>
-      <c r="I17" t="s"/>
-      <c r="J17" t="s"/>
-      <c r="K17" t="s"/>
-      <c r="L17" t="s"/>
+      <c r="A17" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>83</v>
+      </c>
+      <c r="K17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" t="n">
+        <v>11</v>
+      </c>
       <c r="M17" t="s"/>
-      <c r="N17" t="s"/>
-      <c r="O17" t="s"/>
-      <c r="P17" t="s"/>
-      <c r="Q17" t="s"/>
-      <c r="R17" t="s"/>
+      <c r="N17" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17" t="n">
+        <v>3</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
       <c r="S17" t="s"/>
       <c r="T17" t="s"/>
       <c r="U17" t="s"/>
@@ -1663,24 +2084,58 @@
       <c r="AL17" t="s"/>
     </row>
     <row r="18" spans="1:38">
-      <c r="A18" t="s"/>
-      <c r="B18" t="s"/>
-      <c r="C18" t="s"/>
-      <c r="D18" t="s"/>
-      <c r="E18" t="s"/>
-      <c r="F18" t="s"/>
-      <c r="G18" t="s"/>
-      <c r="H18" t="s"/>
-      <c r="I18" t="s"/>
-      <c r="J18" t="s"/>
-      <c r="K18" t="s"/>
-      <c r="L18" t="s"/>
+      <c r="A18" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J18" t="n">
+        <v>83</v>
+      </c>
+      <c r="K18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" t="n">
+        <v>10</v>
+      </c>
       <c r="M18" t="s"/>
-      <c r="N18" t="s"/>
-      <c r="O18" t="s"/>
-      <c r="P18" t="s"/>
-      <c r="Q18" t="s"/>
-      <c r="R18" t="s"/>
+      <c r="N18" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" t="n">
+        <v>3</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
       <c r="S18" t="s"/>
       <c r="T18" t="s"/>
       <c r="U18" t="s"/>
@@ -1703,24 +2158,58 @@
       <c r="AL18" t="s"/>
     </row>
     <row r="19" spans="1:38">
-      <c r="A19" t="s"/>
-      <c r="B19" t="s"/>
-      <c r="C19" t="s"/>
-      <c r="D19" t="s"/>
-      <c r="E19" t="s"/>
-      <c r="F19" t="s"/>
-      <c r="G19" t="s"/>
-      <c r="H19" t="s"/>
-      <c r="I19" t="s"/>
-      <c r="J19" t="s"/>
-      <c r="K19" t="s"/>
-      <c r="L19" t="s"/>
+      <c r="A19" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" t="n">
+        <v>4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" t="n">
+        <v>10</v>
+      </c>
       <c r="M19" t="s"/>
-      <c r="N19" t="s"/>
-      <c r="O19" t="s"/>
-      <c r="P19" t="s"/>
-      <c r="Q19" t="s"/>
-      <c r="R19" t="s"/>
+      <c r="N19" t="s">
+        <v>69</v>
+      </c>
+      <c r="O19" t="n">
+        <v>3</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
       <c r="S19" t="s"/>
       <c r="T19" t="s"/>
       <c r="U19" t="s"/>
@@ -1743,24 +2232,58 @@
       <c r="AL19" t="s"/>
     </row>
     <row r="20" spans="1:38">
-      <c r="A20" t="s"/>
-      <c r="B20" t="s"/>
-      <c r="C20" t="s"/>
-      <c r="D20" t="s"/>
-      <c r="E20" t="s"/>
-      <c r="F20" t="s"/>
-      <c r="G20" t="s"/>
-      <c r="H20" t="s"/>
-      <c r="I20" t="s"/>
-      <c r="J20" t="s"/>
-      <c r="K20" t="s"/>
-      <c r="L20" t="s"/>
+      <c r="A20" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J20" t="n">
+        <v>79</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="n">
+        <v>10</v>
+      </c>
       <c r="M20" t="s"/>
-      <c r="N20" t="s"/>
-      <c r="O20" t="s"/>
-      <c r="P20" t="s"/>
-      <c r="Q20" t="s"/>
-      <c r="R20" t="s"/>
+      <c r="N20" t="s">
+        <v>86</v>
+      </c>
+      <c r="O20" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
       <c r="S20" t="s"/>
       <c r="T20" t="s"/>
       <c r="U20" t="s"/>
@@ -1783,24 +2306,58 @@
       <c r="AL20" t="s"/>
     </row>
     <row r="21" spans="1:38">
-      <c r="A21" t="s"/>
-      <c r="B21" t="s"/>
-      <c r="C21" t="s"/>
-      <c r="D21" t="s"/>
-      <c r="E21" t="s"/>
-      <c r="F21" t="s"/>
-      <c r="G21" t="s"/>
-      <c r="H21" t="s"/>
-      <c r="I21" t="s"/>
-      <c r="J21" t="s"/>
-      <c r="K21" t="s"/>
-      <c r="L21" t="s"/>
+      <c r="A21" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J21" t="n">
+        <v>79</v>
+      </c>
+      <c r="K21" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" t="n">
+        <v>10</v>
+      </c>
       <c r="M21" t="s"/>
-      <c r="N21" t="s"/>
-      <c r="O21" t="s"/>
-      <c r="P21" t="s"/>
-      <c r="Q21" t="s"/>
-      <c r="R21" t="s"/>
+      <c r="N21" t="s">
+        <v>88</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
       <c r="S21" t="s"/>
       <c r="T21" t="s"/>
       <c r="U21" t="s"/>
@@ -1823,24 +2380,58 @@
       <c r="AL21" t="s"/>
     </row>
     <row r="22" spans="1:38">
-      <c r="A22" t="s"/>
-      <c r="B22" t="s"/>
-      <c r="C22" t="s"/>
-      <c r="D22" t="s"/>
-      <c r="E22" t="s"/>
-      <c r="F22" t="s"/>
-      <c r="G22" t="s"/>
-      <c r="H22" t="s"/>
-      <c r="I22" t="s"/>
-      <c r="J22" t="s"/>
-      <c r="K22" t="s"/>
-      <c r="L22" t="s"/>
+      <c r="A22" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J22" t="n">
+        <v>83</v>
+      </c>
+      <c r="K22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10</v>
+      </c>
       <c r="M22" t="s"/>
-      <c r="N22" t="s"/>
-      <c r="O22" t="s"/>
-      <c r="P22" t="s"/>
-      <c r="Q22" t="s"/>
-      <c r="R22" t="s"/>
+      <c r="N22" t="s">
+        <v>90</v>
+      </c>
+      <c r="O22" t="n">
+        <v>3</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
       <c r="S22" t="s"/>
       <c r="T22" t="s"/>
       <c r="U22" t="s"/>
@@ -1863,24 +2454,58 @@
       <c r="AL22" t="s"/>
     </row>
     <row r="23" spans="1:38">
-      <c r="A23" t="s"/>
-      <c r="B23" t="s"/>
-      <c r="C23" t="s"/>
-      <c r="D23" t="s"/>
-      <c r="E23" t="s"/>
-      <c r="F23" t="s"/>
-      <c r="G23" t="s"/>
-      <c r="H23" t="s"/>
-      <c r="I23" t="s"/>
-      <c r="J23" t="s"/>
-      <c r="K23" t="s"/>
-      <c r="L23" t="s"/>
+      <c r="A23" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" t="n">
+        <v>86</v>
+      </c>
+      <c r="K23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" t="n">
+        <v>10</v>
+      </c>
       <c r="M23" t="s"/>
-      <c r="N23" t="s"/>
-      <c r="O23" t="s"/>
-      <c r="P23" t="s"/>
-      <c r="Q23" t="s"/>
-      <c r="R23" t="s"/>
+      <c r="N23" t="s">
+        <v>92</v>
+      </c>
+      <c r="O23" t="n">
+        <v>3</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
       <c r="S23" t="s"/>
       <c r="T23" t="s"/>
       <c r="U23" t="s"/>
@@ -1903,24 +2528,58 @@
       <c r="AL23" t="s"/>
     </row>
     <row r="24" spans="1:38">
-      <c r="A24" t="s"/>
-      <c r="B24" t="s"/>
-      <c r="C24" t="s"/>
-      <c r="D24" t="s"/>
-      <c r="E24" t="s"/>
-      <c r="F24" t="s"/>
-      <c r="G24" t="s"/>
-      <c r="H24" t="s"/>
-      <c r="I24" t="s"/>
-      <c r="J24" t="s"/>
-      <c r="K24" t="s"/>
-      <c r="L24" t="s"/>
+      <c r="A24" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J24" t="n">
+        <v>83</v>
+      </c>
+      <c r="K24" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" t="n">
+        <v>10</v>
+      </c>
       <c r="M24" t="s"/>
-      <c r="N24" t="s"/>
-      <c r="O24" t="s"/>
-      <c r="P24" t="s"/>
-      <c r="Q24" t="s"/>
-      <c r="R24" t="s"/>
+      <c r="N24" t="s">
+        <v>94</v>
+      </c>
+      <c r="O24" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
       <c r="S24" t="s"/>
       <c r="T24" t="s"/>
       <c r="U24" t="s"/>
@@ -1943,24 +2602,58 @@
       <c r="AL24" t="s"/>
     </row>
     <row r="25" spans="1:38">
-      <c r="A25" t="s"/>
-      <c r="B25" t="s"/>
-      <c r="C25" t="s"/>
-      <c r="D25" t="s"/>
-      <c r="E25" t="s"/>
-      <c r="F25" t="s"/>
-      <c r="G25" t="s"/>
-      <c r="H25" t="s"/>
-      <c r="I25" t="s"/>
-      <c r="J25" t="s"/>
-      <c r="K25" t="s"/>
-      <c r="L25" t="s"/>
+      <c r="A25" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J25" t="n">
+        <v>93</v>
+      </c>
+      <c r="K25" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" t="n">
+        <v>10</v>
+      </c>
       <c r="M25" t="s"/>
-      <c r="N25" t="s"/>
-      <c r="O25" t="s"/>
-      <c r="P25" t="s"/>
-      <c r="Q25" t="s"/>
-      <c r="R25" t="s"/>
+      <c r="N25" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" t="n">
+        <v>3</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
       <c r="S25" t="s"/>
       <c r="T25" t="s"/>
       <c r="U25" t="s"/>
@@ -1983,24 +2676,58 @@
       <c r="AL25" t="s"/>
     </row>
     <row r="26" spans="1:38">
-      <c r="A26" t="s"/>
-      <c r="B26" t="s"/>
-      <c r="C26" t="s"/>
-      <c r="D26" t="s"/>
-      <c r="E26" t="s"/>
-      <c r="F26" t="s"/>
-      <c r="G26" t="s"/>
-      <c r="H26" t="s"/>
-      <c r="I26" t="s"/>
-      <c r="J26" t="s"/>
-      <c r="K26" t="s"/>
-      <c r="L26" t="s"/>
+      <c r="A26" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J26" t="n">
+        <v>65</v>
+      </c>
+      <c r="K26" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" t="n">
+        <v>9</v>
+      </c>
       <c r="M26" t="s"/>
-      <c r="N26" t="s"/>
-      <c r="O26" t="s"/>
-      <c r="P26" t="s"/>
-      <c r="Q26" t="s"/>
-      <c r="R26" t="s"/>
+      <c r="N26" t="s">
+        <v>101</v>
+      </c>
+      <c r="O26" t="n">
+        <v>3</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
       <c r="S26" t="s"/>
       <c r="T26" t="s"/>
       <c r="U26" t="s"/>
@@ -2023,24 +2750,58 @@
       <c r="AL26" t="s"/>
     </row>
     <row r="27" spans="1:38">
-      <c r="A27" t="s"/>
-      <c r="B27" t="s"/>
-      <c r="C27" t="s"/>
-      <c r="D27" t="s"/>
-      <c r="E27" t="s"/>
-      <c r="F27" t="s"/>
-      <c r="G27" t="s"/>
-      <c r="H27" t="s"/>
-      <c r="I27" t="s"/>
-      <c r="J27" t="s"/>
-      <c r="K27" t="s"/>
-      <c r="L27" t="s"/>
+      <c r="A27" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J27" t="n">
+        <v>93</v>
+      </c>
+      <c r="K27" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" t="n">
+        <v>9</v>
+      </c>
       <c r="M27" t="s"/>
-      <c r="N27" t="s"/>
-      <c r="O27" t="s"/>
-      <c r="P27" t="s"/>
-      <c r="Q27" t="s"/>
-      <c r="R27" t="s"/>
+      <c r="N27" t="s">
+        <v>90</v>
+      </c>
+      <c r="O27" t="n">
+        <v>3</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
       <c r="S27" t="s"/>
       <c r="T27" t="s"/>
       <c r="U27" t="s"/>
@@ -2063,24 +2824,58 @@
       <c r="AL27" t="s"/>
     </row>
     <row r="28" spans="1:38">
-      <c r="A28" t="s"/>
-      <c r="B28" t="s"/>
-      <c r="C28" t="s"/>
-      <c r="D28" t="s"/>
-      <c r="E28" t="s"/>
-      <c r="F28" t="s"/>
-      <c r="G28" t="s"/>
-      <c r="H28" t="s"/>
-      <c r="I28" t="s"/>
-      <c r="J28" t="s"/>
-      <c r="K28" t="s"/>
-      <c r="L28" t="s"/>
+      <c r="A28" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J28" t="n">
+        <v>83</v>
+      </c>
+      <c r="K28" t="s">
+        <v>56</v>
+      </c>
+      <c r="L28" t="n">
+        <v>9</v>
+      </c>
       <c r="M28" t="s"/>
-      <c r="N28" t="s"/>
-      <c r="O28" t="s"/>
-      <c r="P28" t="s"/>
-      <c r="Q28" t="s"/>
-      <c r="R28" t="s"/>
+      <c r="N28" t="s">
+        <v>104</v>
+      </c>
+      <c r="O28" t="n">
+        <v>3</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
       <c r="S28" t="s"/>
       <c r="T28" t="s"/>
       <c r="U28" t="s"/>
@@ -2103,24 +2898,58 @@
       <c r="AL28" t="s"/>
     </row>
     <row r="29" spans="1:38">
-      <c r="A29" t="s"/>
-      <c r="B29" t="s"/>
-      <c r="C29" t="s"/>
-      <c r="D29" t="s"/>
-      <c r="E29" t="s"/>
-      <c r="F29" t="s"/>
-      <c r="G29" t="s"/>
-      <c r="H29" t="s"/>
-      <c r="I29" t="s"/>
-      <c r="J29" t="s"/>
-      <c r="K29" t="s"/>
-      <c r="L29" t="s"/>
+      <c r="A29" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J29" t="n">
+        <v>79</v>
+      </c>
+      <c r="K29" t="s">
+        <v>56</v>
+      </c>
+      <c r="L29" t="n">
+        <v>9</v>
+      </c>
       <c r="M29" t="s"/>
-      <c r="N29" t="s"/>
-      <c r="O29" t="s"/>
-      <c r="P29" t="s"/>
-      <c r="Q29" t="s"/>
-      <c r="R29" t="s"/>
+      <c r="N29" t="s">
+        <v>106</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
       <c r="S29" t="s"/>
       <c r="T29" t="s"/>
       <c r="U29" t="s"/>
@@ -2143,24 +2972,58 @@
       <c r="AL29" t="s"/>
     </row>
     <row r="30" spans="1:38">
-      <c r="A30" t="s"/>
-      <c r="B30" t="s"/>
-      <c r="C30" t="s"/>
-      <c r="D30" t="s"/>
-      <c r="E30" t="s"/>
-      <c r="F30" t="s"/>
-      <c r="G30" t="s"/>
-      <c r="H30" t="s"/>
-      <c r="I30" t="s"/>
-      <c r="J30" t="s"/>
-      <c r="K30" t="s"/>
-      <c r="L30" t="s"/>
+      <c r="A30" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J30" t="n">
+        <v>70</v>
+      </c>
+      <c r="K30" t="s">
+        <v>56</v>
+      </c>
+      <c r="L30" t="n">
+        <v>9</v>
+      </c>
       <c r="M30" t="s"/>
-      <c r="N30" t="s"/>
-      <c r="O30" t="s"/>
-      <c r="P30" t="s"/>
-      <c r="Q30" t="s"/>
-      <c r="R30" t="s"/>
+      <c r="N30" t="s">
+        <v>108</v>
+      </c>
+      <c r="O30" t="n">
+        <v>3</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
       <c r="S30" t="s"/>
       <c r="T30" t="s"/>
       <c r="U30" t="s"/>
@@ -2183,24 +3046,58 @@
       <c r="AL30" t="s"/>
     </row>
     <row r="31" spans="1:38">
-      <c r="A31" t="s"/>
-      <c r="B31" t="s"/>
-      <c r="C31" t="s"/>
-      <c r="D31" t="s"/>
-      <c r="E31" t="s"/>
-      <c r="F31" t="s"/>
-      <c r="G31" t="s"/>
-      <c r="H31" t="s"/>
-      <c r="I31" t="s"/>
-      <c r="J31" t="s"/>
-      <c r="K31" t="s"/>
-      <c r="L31" t="s"/>
+      <c r="A31" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J31" t="n">
+        <v>83</v>
+      </c>
+      <c r="K31" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" t="n">
+        <v>9</v>
+      </c>
       <c r="M31" t="s"/>
-      <c r="N31" t="s"/>
-      <c r="O31" t="s"/>
-      <c r="P31" t="s"/>
-      <c r="Q31" t="s"/>
-      <c r="R31" t="s"/>
+      <c r="N31" t="s">
+        <v>90</v>
+      </c>
+      <c r="O31" t="n">
+        <v>3</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
       <c r="S31" t="s"/>
       <c r="T31" t="s"/>
       <c r="U31" t="s"/>
@@ -2223,24 +3120,58 @@
       <c r="AL31" t="s"/>
     </row>
     <row r="32" spans="1:38">
-      <c r="A32" t="s"/>
-      <c r="B32" t="s"/>
-      <c r="C32" t="s"/>
-      <c r="D32" t="s"/>
-      <c r="E32" t="s"/>
-      <c r="F32" t="s"/>
-      <c r="G32" t="s"/>
-      <c r="H32" t="s"/>
-      <c r="I32" t="s"/>
-      <c r="J32" t="s"/>
-      <c r="K32" t="s"/>
-      <c r="L32" t="s"/>
+      <c r="A32" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J32" t="n">
+        <v>93</v>
+      </c>
+      <c r="K32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" t="n">
+        <v>9</v>
+      </c>
       <c r="M32" t="s"/>
-      <c r="N32" t="s"/>
-      <c r="O32" t="s"/>
-      <c r="P32" t="s"/>
-      <c r="Q32" t="s"/>
-      <c r="R32" t="s"/>
+      <c r="N32" t="s">
+        <v>92</v>
+      </c>
+      <c r="O32" t="n">
+        <v>3</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
       <c r="S32" t="s"/>
       <c r="T32" t="s"/>
       <c r="U32" t="s"/>
@@ -2263,24 +3194,58 @@
       <c r="AL32" t="s"/>
     </row>
     <row r="33" spans="1:38">
-      <c r="A33" t="s"/>
-      <c r="B33" t="s"/>
-      <c r="C33" t="s"/>
-      <c r="D33" t="s"/>
-      <c r="E33" t="s"/>
-      <c r="F33" t="s"/>
-      <c r="G33" t="s"/>
-      <c r="H33" t="s"/>
-      <c r="I33" t="s"/>
-      <c r="J33" t="s"/>
-      <c r="K33" t="s"/>
-      <c r="L33" t="s"/>
+      <c r="A33" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J33" t="n">
+        <v>70</v>
+      </c>
+      <c r="K33" t="s">
+        <v>56</v>
+      </c>
+      <c r="L33" t="n">
+        <v>9</v>
+      </c>
       <c r="M33" t="s"/>
-      <c r="N33" t="s"/>
-      <c r="O33" t="s"/>
-      <c r="P33" t="s"/>
-      <c r="Q33" t="s"/>
-      <c r="R33" t="s"/>
+      <c r="N33" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" t="n">
+        <v>3</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
       <c r="S33" t="s"/>
       <c r="T33" t="s"/>
       <c r="U33" t="s"/>
@@ -2303,24 +3268,58 @@
       <c r="AL33" t="s"/>
     </row>
     <row r="34" spans="1:38">
-      <c r="A34" t="s"/>
-      <c r="B34" t="s"/>
-      <c r="C34" t="s"/>
-      <c r="D34" t="s"/>
-      <c r="E34" t="s"/>
-      <c r="F34" t="s"/>
-      <c r="G34" t="s"/>
-      <c r="H34" t="s"/>
-      <c r="I34" t="s"/>
-      <c r="J34" t="s"/>
-      <c r="K34" t="s"/>
-      <c r="L34" t="s"/>
+      <c r="A34" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E34" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J34" t="n">
+        <v>93</v>
+      </c>
+      <c r="K34" t="s">
+        <v>56</v>
+      </c>
+      <c r="L34" t="n">
+        <v>9</v>
+      </c>
       <c r="M34" t="s"/>
-      <c r="N34" t="s"/>
-      <c r="O34" t="s"/>
-      <c r="P34" t="s"/>
-      <c r="Q34" t="s"/>
-      <c r="R34" t="s"/>
+      <c r="N34" t="s">
+        <v>114</v>
+      </c>
+      <c r="O34" t="n">
+        <v>3</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
       <c r="S34" t="s"/>
       <c r="T34" t="s"/>
       <c r="U34" t="s"/>
@@ -2343,24 +3342,58 @@
       <c r="AL34" t="s"/>
     </row>
     <row r="35" spans="1:38">
-      <c r="A35" t="s"/>
-      <c r="B35" t="s"/>
-      <c r="C35" t="s"/>
-      <c r="D35" t="s"/>
-      <c r="E35" t="s"/>
-      <c r="F35" t="s"/>
-      <c r="G35" t="s"/>
-      <c r="H35" t="s"/>
-      <c r="I35" t="s"/>
-      <c r="J35" t="s"/>
-      <c r="K35" t="s"/>
-      <c r="L35" t="s"/>
+      <c r="A35" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" t="s">
+        <v>100</v>
+      </c>
+      <c r="I35" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J35" t="n">
+        <v>100</v>
+      </c>
+      <c r="K35" t="s">
+        <v>56</v>
+      </c>
+      <c r="L35" t="n">
+        <v>9</v>
+      </c>
       <c r="M35" t="s"/>
-      <c r="N35" t="s"/>
-      <c r="O35" t="s"/>
-      <c r="P35" t="s"/>
-      <c r="Q35" t="s"/>
-      <c r="R35" t="s"/>
+      <c r="N35" t="s">
+        <v>117</v>
+      </c>
+      <c r="O35" t="n">
+        <v>3</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
       <c r="S35" t="s"/>
       <c r="T35" t="s"/>
       <c r="U35" t="s"/>
@@ -2383,24 +3416,58 @@
       <c r="AL35" t="s"/>
     </row>
     <row r="36" spans="1:38">
-      <c r="A36" t="s"/>
-      <c r="B36" t="s"/>
-      <c r="C36" t="s"/>
-      <c r="D36" t="s"/>
-      <c r="E36" t="s"/>
-      <c r="F36" t="s"/>
-      <c r="G36" t="s"/>
-      <c r="H36" t="s"/>
-      <c r="I36" t="s"/>
-      <c r="J36" t="s"/>
-      <c r="K36" t="s"/>
-      <c r="L36" t="s"/>
+      <c r="A36" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" t="s">
+        <v>119</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4</v>
+      </c>
+      <c r="J36" t="n">
+        <v>96</v>
+      </c>
+      <c r="K36" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" t="n">
+        <v>8</v>
+      </c>
       <c r="M36" t="s"/>
-      <c r="N36" t="s"/>
-      <c r="O36" t="s"/>
-      <c r="P36" t="s"/>
-      <c r="Q36" t="s"/>
-      <c r="R36" t="s"/>
+      <c r="N36" t="s">
+        <v>120</v>
+      </c>
+      <c r="O36" t="n">
+        <v>3</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
       <c r="S36" t="s"/>
       <c r="T36" t="s"/>
       <c r="U36" t="s"/>
@@ -2423,24 +3490,58 @@
       <c r="AL36" t="s"/>
     </row>
     <row r="37" spans="1:38">
-      <c r="A37" t="s"/>
-      <c r="B37" t="s"/>
-      <c r="C37" t="s"/>
-      <c r="D37" t="s"/>
-      <c r="E37" t="s"/>
-      <c r="F37" t="s"/>
-      <c r="G37" t="s"/>
-      <c r="H37" t="s"/>
-      <c r="I37" t="s"/>
-      <c r="J37" t="s"/>
-      <c r="K37" t="s"/>
-      <c r="L37" t="s"/>
+      <c r="A37" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2</v>
+      </c>
+      <c r="J37" t="n">
+        <v>75</v>
+      </c>
+      <c r="K37" t="s">
+        <v>56</v>
+      </c>
+      <c r="L37" t="n">
+        <v>8</v>
+      </c>
       <c r="M37" t="s"/>
-      <c r="N37" t="s"/>
-      <c r="O37" t="s"/>
-      <c r="P37" t="s"/>
-      <c r="Q37" t="s"/>
-      <c r="R37" t="s"/>
+      <c r="N37" t="s">
+        <v>122</v>
+      </c>
+      <c r="O37" t="n">
+        <v>3</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
       <c r="S37" t="s"/>
       <c r="T37" t="s"/>
       <c r="U37" t="s"/>
@@ -2463,24 +3564,58 @@
       <c r="AL37" t="s"/>
     </row>
     <row r="38" spans="1:38">
-      <c r="A38" t="s"/>
-      <c r="B38" t="s"/>
-      <c r="C38" t="s"/>
-      <c r="D38" t="s"/>
-      <c r="E38" t="s"/>
-      <c r="F38" t="s"/>
-      <c r="G38" t="s"/>
-      <c r="H38" t="s"/>
-      <c r="I38" t="s"/>
-      <c r="J38" t="s"/>
-      <c r="K38" t="s"/>
-      <c r="L38" t="s"/>
+      <c r="A38" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>119</v>
+      </c>
+      <c r="I38" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J38" t="n">
+        <v>93</v>
+      </c>
+      <c r="K38" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" t="n">
+        <v>8</v>
+      </c>
       <c r="M38" t="s"/>
-      <c r="N38" t="s"/>
-      <c r="O38" t="s"/>
-      <c r="P38" t="s"/>
-      <c r="Q38" t="s"/>
-      <c r="R38" t="s"/>
+      <c r="N38" t="s">
+        <v>124</v>
+      </c>
+      <c r="O38" t="n">
+        <v>3</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
       <c r="S38" t="s"/>
       <c r="T38" t="s"/>
       <c r="U38" t="s"/>
@@ -2503,24 +3638,58 @@
       <c r="AL38" t="s"/>
     </row>
     <row r="39" spans="1:38">
-      <c r="A39" t="s"/>
-      <c r="B39" t="s"/>
-      <c r="C39" t="s"/>
-      <c r="D39" t="s"/>
-      <c r="E39" t="s"/>
-      <c r="F39" t="s"/>
-      <c r="G39" t="s"/>
-      <c r="H39" t="s"/>
-      <c r="I39" t="s"/>
-      <c r="J39" t="s"/>
-      <c r="K39" t="s"/>
-      <c r="L39" t="s"/>
+      <c r="A39" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" t="n">
+        <v>3</v>
+      </c>
+      <c r="J39" t="n">
+        <v>86</v>
+      </c>
+      <c r="K39" t="s">
+        <v>56</v>
+      </c>
+      <c r="L39" t="n">
+        <v>8</v>
+      </c>
       <c r="M39" t="s"/>
-      <c r="N39" t="s"/>
-      <c r="O39" t="s"/>
-      <c r="P39" t="s"/>
-      <c r="Q39" t="s"/>
-      <c r="R39" t="s"/>
+      <c r="N39" t="s">
+        <v>106</v>
+      </c>
+      <c r="O39" t="n">
+        <v>3</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
       <c r="S39" t="s"/>
       <c r="T39" t="s"/>
       <c r="U39" t="s"/>
@@ -2543,24 +3712,58 @@
       <c r="AL39" t="s"/>
     </row>
     <row r="40" spans="1:38">
-      <c r="A40" t="s"/>
-      <c r="B40" t="s"/>
-      <c r="C40" t="s"/>
-      <c r="D40" t="s"/>
-      <c r="E40" t="s"/>
-      <c r="F40" t="s"/>
-      <c r="G40" t="s"/>
-      <c r="H40" t="s"/>
-      <c r="I40" t="s"/>
-      <c r="J40" t="s"/>
-      <c r="K40" t="s"/>
-      <c r="L40" t="s"/>
+      <c r="A40" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s">
+        <v>119</v>
+      </c>
+      <c r="I40" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J40" t="n">
+        <v>83</v>
+      </c>
+      <c r="K40" t="s">
+        <v>56</v>
+      </c>
+      <c r="L40" t="n">
+        <v>8</v>
+      </c>
       <c r="M40" t="s"/>
-      <c r="N40" t="s"/>
-      <c r="O40" t="s"/>
-      <c r="P40" t="s"/>
-      <c r="Q40" t="s"/>
-      <c r="R40" t="s"/>
+      <c r="N40" t="s">
+        <v>127</v>
+      </c>
+      <c r="O40" t="n">
+        <v>3</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
       <c r="S40" t="s"/>
       <c r="T40" t="s"/>
       <c r="U40" t="s"/>
@@ -2583,24 +3786,58 @@
       <c r="AL40" t="s"/>
     </row>
     <row r="41" spans="1:38">
-      <c r="A41" t="s"/>
-      <c r="B41" t="s"/>
-      <c r="C41" t="s"/>
-      <c r="D41" t="s"/>
-      <c r="E41" t="s"/>
-      <c r="F41" t="s"/>
-      <c r="G41" t="s"/>
-      <c r="H41" t="s"/>
-      <c r="I41" t="s"/>
-      <c r="J41" t="s"/>
-      <c r="K41" t="s"/>
-      <c r="L41" t="s"/>
+      <c r="A41" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>119</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+      <c r="J41" t="n">
+        <v>86</v>
+      </c>
+      <c r="K41" t="s">
+        <v>56</v>
+      </c>
+      <c r="L41" t="n">
+        <v>8</v>
+      </c>
       <c r="M41" t="s"/>
-      <c r="N41" t="s"/>
-      <c r="O41" t="s"/>
-      <c r="P41" t="s"/>
-      <c r="Q41" t="s"/>
-      <c r="R41" t="s"/>
+      <c r="N41" t="s">
+        <v>120</v>
+      </c>
+      <c r="O41" t="n">
+        <v>3</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
       <c r="S41" t="s"/>
       <c r="T41" t="s"/>
       <c r="U41" t="s"/>
@@ -2623,24 +3860,58 @@
       <c r="AL41" t="s"/>
     </row>
     <row r="42" spans="1:38">
-      <c r="A42" t="s"/>
-      <c r="B42" t="s"/>
-      <c r="C42" t="s"/>
-      <c r="D42" t="s"/>
-      <c r="E42" t="s"/>
-      <c r="F42" t="s"/>
-      <c r="G42" t="s"/>
-      <c r="H42" t="s"/>
-      <c r="I42" t="s"/>
-      <c r="J42" t="s"/>
-      <c r="K42" t="s"/>
-      <c r="L42" t="s"/>
+      <c r="A42" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" t="s">
+        <v>119</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
+      </c>
+      <c r="J42" t="n">
+        <v>86</v>
+      </c>
+      <c r="K42" t="s">
+        <v>56</v>
+      </c>
+      <c r="L42" t="n">
+        <v>8</v>
+      </c>
       <c r="M42" t="s"/>
-      <c r="N42" t="s"/>
-      <c r="O42" t="s"/>
-      <c r="P42" t="s"/>
-      <c r="Q42" t="s"/>
-      <c r="R42" t="s"/>
+      <c r="N42" t="s">
+        <v>92</v>
+      </c>
+      <c r="O42" t="n">
+        <v>3</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
       <c r="S42" t="s"/>
       <c r="T42" t="s"/>
       <c r="U42" t="s"/>
@@ -2663,24 +3934,58 @@
       <c r="AL42" t="s"/>
     </row>
     <row r="43" spans="1:38">
-      <c r="A43" t="s"/>
-      <c r="B43" t="s"/>
-      <c r="C43" t="s"/>
-      <c r="D43" t="s"/>
-      <c r="E43" t="s"/>
-      <c r="F43" t="s"/>
-      <c r="G43" t="s"/>
-      <c r="H43" t="s"/>
-      <c r="I43" t="s"/>
-      <c r="J43" t="s"/>
-      <c r="K43" t="s"/>
-      <c r="L43" t="s"/>
+      <c r="A43" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3</v>
+      </c>
+      <c r="J43" t="n">
+        <v>86</v>
+      </c>
+      <c r="K43" t="s">
+        <v>56</v>
+      </c>
+      <c r="L43" t="n">
+        <v>8</v>
+      </c>
       <c r="M43" t="s"/>
-      <c r="N43" t="s"/>
-      <c r="O43" t="s"/>
-      <c r="P43" t="s"/>
-      <c r="Q43" t="s"/>
-      <c r="R43" t="s"/>
+      <c r="N43" t="s">
+        <v>131</v>
+      </c>
+      <c r="O43" t="n">
+        <v>3</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
       <c r="S43" t="s"/>
       <c r="T43" t="s"/>
       <c r="U43" t="s"/>
@@ -2703,24 +4008,58 @@
       <c r="AL43" t="s"/>
     </row>
     <row r="44" spans="1:38">
-      <c r="A44" t="s"/>
-      <c r="B44" t="s"/>
-      <c r="C44" t="s"/>
-      <c r="D44" t="s"/>
-      <c r="E44" t="s"/>
-      <c r="F44" t="s"/>
-      <c r="G44" t="s"/>
-      <c r="H44" t="s"/>
-      <c r="I44" t="s"/>
-      <c r="J44" t="s"/>
-      <c r="K44" t="s"/>
-      <c r="L44" t="s"/>
+      <c r="A44" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H44" t="s">
+        <v>119</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J44" t="n">
+        <v>65</v>
+      </c>
+      <c r="K44" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" t="n">
+        <v>8</v>
+      </c>
       <c r="M44" t="s"/>
-      <c r="N44" t="s"/>
-      <c r="O44" t="s"/>
-      <c r="P44" t="s"/>
-      <c r="Q44" t="s"/>
-      <c r="R44" t="s"/>
+      <c r="N44" t="s">
+        <v>133</v>
+      </c>
+      <c r="O44" t="n">
+        <v>3</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
       <c r="S44" t="s"/>
       <c r="T44" t="s"/>
       <c r="U44" t="s"/>
@@ -2743,24 +4082,58 @@
       <c r="AL44" t="s"/>
     </row>
     <row r="45" spans="1:38">
-      <c r="A45" t="s"/>
-      <c r="B45" t="s"/>
-      <c r="C45" t="s"/>
-      <c r="D45" t="s"/>
-      <c r="E45" t="s"/>
-      <c r="F45" t="s"/>
-      <c r="G45" t="s"/>
-      <c r="H45" t="s"/>
-      <c r="I45" t="s"/>
-      <c r="J45" t="s"/>
-      <c r="K45" t="s"/>
-      <c r="L45" t="s"/>
+      <c r="A45" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" t="s">
+        <v>119</v>
+      </c>
+      <c r="I45" t="n">
+        <v>4</v>
+      </c>
+      <c r="J45" t="n">
+        <v>96</v>
+      </c>
+      <c r="K45" t="s">
+        <v>56</v>
+      </c>
+      <c r="L45" t="n">
+        <v>8</v>
+      </c>
       <c r="M45" t="s"/>
-      <c r="N45" t="s"/>
-      <c r="O45" t="s"/>
-      <c r="P45" t="s"/>
-      <c r="Q45" t="s"/>
-      <c r="R45" t="s"/>
+      <c r="N45" t="s">
+        <v>97</v>
+      </c>
+      <c r="O45" t="n">
+        <v>3</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
       <c r="S45" t="s"/>
       <c r="T45" t="s"/>
       <c r="U45" t="s"/>
@@ -2783,24 +4156,58 @@
       <c r="AL45" t="s"/>
     </row>
     <row r="46" spans="1:38">
-      <c r="A46" t="s"/>
-      <c r="B46" t="s"/>
-      <c r="C46" t="s"/>
-      <c r="D46" t="s"/>
-      <c r="E46" t="s"/>
-      <c r="F46" t="s"/>
-      <c r="G46" t="s"/>
-      <c r="H46" t="s"/>
-      <c r="I46" t="s"/>
-      <c r="J46" t="s"/>
-      <c r="K46" t="s"/>
-      <c r="L46" t="s"/>
+      <c r="A46" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>116</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="s">
+        <v>119</v>
+      </c>
+      <c r="I46" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J46" t="n">
+        <v>100</v>
+      </c>
+      <c r="K46" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" t="n">
+        <v>8</v>
+      </c>
       <c r="M46" t="s"/>
-      <c r="N46" t="s"/>
-      <c r="O46" t="s"/>
-      <c r="P46" t="s"/>
-      <c r="Q46" t="s"/>
-      <c r="R46" t="s"/>
+      <c r="N46" t="s">
+        <v>136</v>
+      </c>
+      <c r="O46" t="n">
+        <v>3</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
       <c r="S46" t="s"/>
       <c r="T46" t="s"/>
       <c r="U46" t="s"/>
@@ -2823,24 +4230,56 @@
       <c r="AL46" t="s"/>
     </row>
     <row r="47" spans="1:38">
-      <c r="A47" t="s"/>
-      <c r="B47" t="s"/>
-      <c r="C47" t="s"/>
-      <c r="D47" t="s"/>
-      <c r="E47" t="s"/>
-      <c r="F47" t="s"/>
-      <c r="G47" t="s"/>
-      <c r="H47" t="s"/>
-      <c r="I47" t="s"/>
-      <c r="J47" t="s"/>
-      <c r="K47" t="s"/>
-      <c r="L47" t="s"/>
+      <c r="A47" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47" t="s">
+        <v>138</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J47" t="n">
+        <v>70</v>
+      </c>
+      <c r="K47" t="s">
+        <v>56</v>
+      </c>
+      <c r="L47" t="n">
+        <v>7</v>
+      </c>
       <c r="M47" t="s"/>
       <c r="N47" t="s"/>
-      <c r="O47" t="s"/>
-      <c r="P47" t="s"/>
-      <c r="Q47" t="s"/>
-      <c r="R47" t="s"/>
+      <c r="O47" t="n">
+        <v>3</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
       <c r="S47" t="s"/>
       <c r="T47" t="s"/>
       <c r="U47" t="s"/>
@@ -2863,24 +4302,56 @@
       <c r="AL47" t="s"/>
     </row>
     <row r="48" spans="1:38">
-      <c r="A48" t="s"/>
-      <c r="B48" t="s"/>
-      <c r="C48" t="s"/>
-      <c r="D48" t="s"/>
-      <c r="E48" t="s"/>
-      <c r="F48" t="s"/>
-      <c r="G48" t="s"/>
-      <c r="H48" t="s"/>
-      <c r="I48" t="s"/>
-      <c r="J48" t="s"/>
-      <c r="K48" t="s"/>
-      <c r="L48" t="s"/>
+      <c r="A48" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H48" t="s">
+        <v>138</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J48" t="n">
+        <v>70</v>
+      </c>
+      <c r="K48" t="s">
+        <v>56</v>
+      </c>
+      <c r="L48" t="n">
+        <v>7</v>
+      </c>
       <c r="M48" t="s"/>
       <c r="N48" t="s"/>
-      <c r="O48" t="s"/>
-      <c r="P48" t="s"/>
-      <c r="Q48" t="s"/>
-      <c r="R48" t="s"/>
+      <c r="O48" t="n">
+        <v>3</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
       <c r="S48" t="s"/>
       <c r="T48" t="s"/>
       <c r="U48" t="s"/>
@@ -2903,24 +4374,56 @@
       <c r="AL48" t="s"/>
     </row>
     <row r="49" spans="1:38">
-      <c r="A49" t="s"/>
-      <c r="B49" t="s"/>
-      <c r="C49" t="s"/>
-      <c r="D49" t="s"/>
-      <c r="E49" t="s"/>
-      <c r="F49" t="s"/>
-      <c r="G49" t="s"/>
-      <c r="H49" t="s"/>
-      <c r="I49" t="s"/>
-      <c r="J49" t="s"/>
-      <c r="K49" t="s"/>
-      <c r="L49" t="s"/>
+      <c r="A49" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" t="s">
+        <v>138</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="n">
+        <v>60</v>
+      </c>
+      <c r="K49" t="s">
+        <v>56</v>
+      </c>
+      <c r="L49" t="n">
+        <v>7</v>
+      </c>
       <c r="M49" t="s"/>
       <c r="N49" t="s"/>
-      <c r="O49" t="s"/>
-      <c r="P49" t="s"/>
-      <c r="Q49" t="s"/>
-      <c r="R49" t="s"/>
+      <c r="O49" t="n">
+        <v>3</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
       <c r="S49" t="s"/>
       <c r="T49" t="s"/>
       <c r="U49" t="s"/>
@@ -2943,24 +4446,56 @@
       <c r="AL49" t="s"/>
     </row>
     <row r="50" spans="1:38">
-      <c r="A50" t="s"/>
-      <c r="B50" t="s"/>
-      <c r="C50" t="s"/>
-      <c r="D50" t="s"/>
-      <c r="E50" t="s"/>
-      <c r="F50" t="s"/>
-      <c r="G50" t="s"/>
-      <c r="H50" t="s"/>
-      <c r="I50" t="s"/>
-      <c r="J50" t="s"/>
-      <c r="K50" t="s"/>
-      <c r="L50" t="s"/>
+      <c r="A50" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50" t="s">
+        <v>138</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J50" t="n">
+        <v>70</v>
+      </c>
+      <c r="K50" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50" t="n">
+        <v>7</v>
+      </c>
       <c r="M50" t="s"/>
       <c r="N50" t="s"/>
-      <c r="O50" t="s"/>
-      <c r="P50" t="s"/>
-      <c r="Q50" t="s"/>
-      <c r="R50" t="s"/>
+      <c r="O50" t="n">
+        <v>3</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
       <c r="S50" t="s"/>
       <c r="T50" t="s"/>
       <c r="U50" t="s"/>
@@ -2983,24 +4518,56 @@
       <c r="AL50" t="s"/>
     </row>
     <row r="51" spans="1:38">
-      <c r="A51" t="s"/>
-      <c r="B51" t="s"/>
-      <c r="C51" t="s"/>
-      <c r="D51" t="s"/>
-      <c r="E51" t="s"/>
-      <c r="F51" t="s"/>
-      <c r="G51" t="s"/>
-      <c r="H51" t="s"/>
-      <c r="I51" t="s"/>
-      <c r="J51" t="s"/>
-      <c r="K51" t="s"/>
-      <c r="L51" t="s"/>
+      <c r="A51" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" t="s">
+        <v>138</v>
+      </c>
+      <c r="I51" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J51" t="n">
+        <v>70</v>
+      </c>
+      <c r="K51" t="s">
+        <v>56</v>
+      </c>
+      <c r="L51" t="n">
+        <v>7</v>
+      </c>
       <c r="M51" t="s"/>
       <c r="N51" t="s"/>
-      <c r="O51" t="s"/>
-      <c r="P51" t="s"/>
-      <c r="Q51" t="s"/>
-      <c r="R51" t="s"/>
+      <c r="O51" t="n">
+        <v>3</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
       <c r="S51" t="s"/>
       <c r="T51" t="s"/>
       <c r="U51" t="s"/>
@@ -3023,24 +4590,56 @@
       <c r="AL51" t="s"/>
     </row>
     <row r="52" spans="1:38">
-      <c r="A52" t="s"/>
-      <c r="B52" t="s"/>
-      <c r="C52" t="s"/>
-      <c r="D52" t="s"/>
-      <c r="E52" t="s"/>
-      <c r="F52" t="s"/>
-      <c r="G52" t="s"/>
-      <c r="H52" t="s"/>
-      <c r="I52" t="s"/>
-      <c r="J52" t="s"/>
-      <c r="K52" t="s"/>
-      <c r="L52" t="s"/>
+      <c r="A52" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>54</v>
+      </c>
+      <c r="H52" t="s">
+        <v>138</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J52" t="n">
+        <v>70</v>
+      </c>
+      <c r="K52" t="s">
+        <v>56</v>
+      </c>
+      <c r="L52" t="n">
+        <v>7</v>
+      </c>
       <c r="M52" t="s"/>
       <c r="N52" t="s"/>
-      <c r="O52" t="s"/>
-      <c r="P52" t="s"/>
-      <c r="Q52" t="s"/>
-      <c r="R52" t="s"/>
+      <c r="O52" t="n">
+        <v>3</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
       <c r="S52" t="s"/>
       <c r="T52" t="s"/>
       <c r="U52" t="s"/>
@@ -3063,24 +4662,56 @@
       <c r="AL52" t="s"/>
     </row>
     <row r="53" spans="1:38">
-      <c r="A53" t="s"/>
-      <c r="B53" t="s"/>
-      <c r="C53" t="s"/>
-      <c r="D53" t="s"/>
-      <c r="E53" t="s"/>
-      <c r="F53" t="s"/>
-      <c r="G53" t="s"/>
-      <c r="H53" t="s"/>
-      <c r="I53" t="s"/>
-      <c r="J53" t="s"/>
-      <c r="K53" t="s"/>
-      <c r="L53" t="s"/>
+      <c r="A53" t="n">
+        <v>605410</v>
+      </c>
+      <c r="B53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" t="n">
+        <v>70001</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>54</v>
+      </c>
+      <c r="H53" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J53" t="n">
+        <v>70</v>
+      </c>
+      <c r="K53" t="s">
+        <v>56</v>
+      </c>
+      <c r="L53" t="n">
+        <v>7</v>
+      </c>
       <c r="M53" t="s"/>
       <c r="N53" t="s"/>
-      <c r="O53" t="s"/>
-      <c r="P53" t="s"/>
-      <c r="Q53" t="s"/>
-      <c r="R53" t="s"/>
+      <c r="O53" t="n">
+        <v>3</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
       <c r="S53" t="s"/>
       <c r="T53" t="s"/>
       <c r="U53" t="s"/>

</xml_diff>